<commit_message>
funcionalides excel implementadas correctamente
</commit_message>
<xml_diff>
--- a/ListaLibros.xlsx
+++ b/ListaLibros.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juank\Desktop\DAW\Proyectos\Biblioteca-Grupal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740642F9-37B0-4D56-9C05-BB77F2CFC817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749D88B1-4CDC-4833-A11A-692F15ECE833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="876" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Libros" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>NOMBRE LIBRO</t>
-  </si>
   <si>
     <t>AUTOR</t>
   </si>
@@ -36,7 +28,10 @@
     <t>ID</t>
   </si>
   <si>
-    <t>UDS DISPONBLES</t>
+    <t>UDS</t>
+  </si>
+  <si>
+    <t>TITULO</t>
   </si>
 </sst>
 </file>
@@ -46,7 +41,7 @@
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,7 +49,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,7 +64,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -101,16 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -130,7 +119,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -146,7 +135,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -158,7 +147,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -205,6 +194,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -240,6 +246,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,27 +417,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>